<commit_message>
passage Teensy 3.5 + debut lidar
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git folder\my_robot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Folder\my_robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E8FA87-D87F-4EC9-8F73-48592688CB06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E71F9E7-CFEC-49C1-B6C9-A981231C2ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Éléments achetés" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="70">
   <si>
     <t>Description</t>
   </si>
@@ -247,9 +247,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>Carte Teensy 3.6</t>
-  </si>
-  <si>
     <t>Connecteurs</t>
   </si>
   <si>
@@ -272,6 +269,9 @@
   </si>
   <si>
     <t>09705</t>
+  </si>
+  <si>
+    <t>Carte Teensy 3.5</t>
   </si>
 </sst>
 </file>
@@ -282,7 +282,7 @@
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,14 +325,6 @@
       <b/>
       <sz val="18"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -413,7 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -482,8 +474,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -500,24 +505,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -535,10 +524,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -806,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,54 +807,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="31" t="s">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="31" t="s">
+      <c r="C1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="27" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="13" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1023,16 +1008,16 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1044,10 +1029,10 @@
       <c r="E13" s="5">
         <v>0</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F13" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="31">
         <v>100012</v>
       </c>
     </row>
@@ -1063,8 +1048,8 @@
       <c r="E14" s="5">
         <v>0</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="26"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
@@ -1079,8 +1064,8 @@
       <c r="E15" s="16">
         <v>0</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="26"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1094,8 +1079,8 @@
       <c r="E16" s="5">
         <v>0</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="26"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1107,8 +1092,8 @@
       <c r="E17" s="5">
         <v>0</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="26"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
@@ -1122,58 +1107,55 @@
       <c r="E18" s="16">
         <v>0</v>
       </c>
-      <c r="F18" s="28"/>
+      <c r="F18" s="33"/>
       <c r="G18" s="17">
         <v>100315</v>
       </c>
       <c r="H18" s="14"/>
     </row>
     <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B22" s="11">
         <v>1</v>
       </c>
       <c r="C22" s="3">
-        <v>37.9</v>
+        <v>29.7</v>
       </c>
       <c r="D22" s="3">
         <f>C22*B22</f>
-        <v>37.9</v>
-      </c>
-      <c r="E22" s="24">
-        <v>1</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>26</v>
+        <v>29.7</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0</v>
       </c>
       <c r="G22" s="8">
-        <v>34780</v>
+        <v>34778</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1201,20 +1183,20 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
+      <c r="A24" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>60</v>
@@ -1227,15 +1209,15 @@
         <v>0</v>
       </c>
       <c r="F25" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="28" t="s">
         <v>64</v>
-      </c>
-      <c r="G25" s="34" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="11">
         <v>2</v>
@@ -1253,13 +1235,13 @@
       <c r="F26" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="36" t="s">
-        <v>68</v>
+      <c r="G26" s="29" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="11">
         <v>2</v>
@@ -1277,8 +1259,8 @@
       <c r="F27" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="36" t="s">
-        <v>69</v>
+      <c r="G27" s="29" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1299,7 +1281,7 @@
     <hyperlink ref="G8" r:id="rId4" location="complte_desc" display="https://www.gotronic.fr/art-roulement-19-6-6mm-157.htm - complte_desc" xr:uid="{668C1373-B577-40D7-AE22-CEC46B56C596}"/>
     <hyperlink ref="G18" r:id="rId5" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{8FB5AF53-6074-4AC8-B954-48BA8EAD3BBD}"/>
     <hyperlink ref="G4" r:id="rId6" xr:uid="{5695B478-FFC7-41D3-9378-789EA5284F3B}"/>
-    <hyperlink ref="G22" r:id="rId7" display="https://www.gotronic.fr/art-carte-teensy-3-6-25426.htm" xr:uid="{7F61F742-4E65-43DD-B561-497192D7846D}"/>
+    <hyperlink ref="G22" r:id="rId7" display="https://www.gotronic.fr/art-carte-teensy-3-5-25425.htm" xr:uid="{7F61F742-4E65-43DD-B561-497192D7846D}"/>
     <hyperlink ref="G13:G17" r:id="rId8" display="https://www.makerbeam.com/makerbeam-makerbeam-regular-starter-kit-black.html" xr:uid="{CFD83EBE-9F65-4299-92FF-2460DE3F7642}"/>
     <hyperlink ref="G23" r:id="rId9" xr:uid="{686BB581-4F17-4F21-B9CD-225D9D0390C3}"/>
     <hyperlink ref="G25" r:id="rId10" xr:uid="{95571536-5EEA-4D58-947A-37D156F02C8F}"/>
@@ -1332,31 +1314,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="30" t="s">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="27" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1467,10 +1449,10 @@
       <c r="D6" s="5">
         <v>0</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="29"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="1" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
maj bom + design piece lidar
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Folder\my_robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E71F9E7-CFEC-49C1-B6C9-A981231C2ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A682C18F-F36D-43E8-8770-DBE0329027DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,6 +225,39 @@
     </r>
   </si>
   <si>
+    <t>Structure MakerBeam</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Connecteurs</t>
+  </si>
+  <si>
+    <t>Embase à broches Molex, KK 254, 4 pôles</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>483-8483</t>
+  </si>
+  <si>
+    <t>Porte-fusible 5,08mm</t>
+  </si>
+  <si>
+    <t>Fusible rapide 3,15 A</t>
+  </si>
+  <si>
+    <t>09730</t>
+  </si>
+  <si>
+    <t>09705</t>
+  </si>
+  <si>
+    <t>Carte Teensy 3.5</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Codeur rotatif - </t>
     </r>
@@ -237,41 +270,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>NC</t>
+      <t>LPD3806-600BM-G5-24C</t>
     </r>
-  </si>
-  <si>
-    <t>Structure MakerBeam</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Connecteurs</t>
-  </si>
-  <si>
-    <t>Embase à broches Molex, KK 254, 4 pôles</t>
-  </si>
-  <si>
-    <t>RS</t>
-  </si>
-  <si>
-    <t>483-8483</t>
-  </si>
-  <si>
-    <t>Porte-fusible 5,08mm</t>
-  </si>
-  <si>
-    <t>Fusible rapide 3,15 A</t>
-  </si>
-  <si>
-    <t>09730</t>
-  </si>
-  <si>
-    <t>09705</t>
-  </si>
-  <si>
-    <t>Carte Teensy 3.5</t>
   </si>
 </sst>
 </file>
@@ -282,7 +282,7 @@
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,6 +325,14 @@
       <b/>
       <sz val="18"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -405,7 +413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -507,6 +515,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -791,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +894,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B5" s="6">
         <v>2</v>
@@ -896,7 +907,7 @@
         <v>38.380000000000003</v>
       </c>
       <c r="E5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>48</v>
@@ -1009,7 +1020,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
@@ -1100,7 +1111,7 @@
         <v>43</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
@@ -1139,7 +1150,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22" s="11">
         <v>1</v>
@@ -1172,8 +1183,8 @@
         <f>C23*B23</f>
         <v>5</v>
       </c>
-      <c r="E23" s="5">
-        <v>0</v>
+      <c r="E23" s="36">
+        <v>3</v>
       </c>
       <c r="F23" s="11" t="s">
         <v>48</v>
@@ -1184,7 +1195,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="30"/>
       <c r="C24" s="30"/>
@@ -1196,10 +1207,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="3">
         <f>0.328 / 10</f>
@@ -1209,15 +1220,15 @@
         <v>0</v>
       </c>
       <c r="F25" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="28" t="s">
         <v>63</v>
-      </c>
-      <c r="G25" s="28" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" s="11">
         <v>2</v>
@@ -1236,12 +1247,12 @@
         <v>26</v>
       </c>
       <c r="G26" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" s="11">
         <v>2</v>
@@ -1260,7 +1271,7 @@
         <v>26</v>
       </c>
       <c r="G27" s="29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modif elec + meca
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Folder\my_robot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git folder\my_robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8888DE08-FCC9-479B-AC4B-539881E84894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFB845C-6BB4-4465-81B2-B7446085BE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Éléments achetés" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
   <si>
     <t>Description</t>
   </si>
@@ -272,6 +272,12 @@
       </rPr>
       <t>LPD3806-600BM-G5-24C</t>
     </r>
+  </si>
+  <si>
+    <t>Étage Actionneurs</t>
+  </si>
+  <si>
+    <t>Étage Lidar</t>
   </si>
 </sst>
 </file>
@@ -413,7 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -518,6 +524,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -800,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,8 +1085,7 @@
         <v>45</v>
       </c>
       <c r="B15" s="19">
-        <f>4+2</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -1124,21 +1141,31 @@
       </c>
       <c r="H18" s="14"/>
     </row>
-    <row r="20" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="33"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+    </row>
+    <row r="20" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="37"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+    </row>
+    <row r="21" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B21" s="31"/>
       <c r="C21" s="31"/>
@@ -1148,145 +1175,188 @@
       <c r="G21" s="31"/>
       <c r="H21" s="31"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+    <row r="22" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="39">
+        <v>2</v>
+      </c>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="40">
+        <f>E15</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+    </row>
+    <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B26" s="11">
         <v>1</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C26" s="3">
         <v>29.7</v>
       </c>
-      <c r="D22" s="3">
-        <f>C22*B22</f>
+      <c r="D26" s="3">
+        <f>C26*B26</f>
         <v>29.7</v>
       </c>
-      <c r="E22" s="5">
-        <v>0</v>
-      </c>
-      <c r="F22" s="11" t="s">
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G26" s="8">
         <v>34778</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="11">
-        <v>2</v>
-      </c>
-      <c r="C23" s="3">
+      <c r="B27" s="11">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3">
         <v>2.5</v>
       </c>
-      <c r="D23" s="3">
-        <f>C23*B23</f>
+      <c r="D27" s="3">
+        <f>C27*B27</f>
         <v>5</v>
       </c>
-      <c r="E23" s="30">
+      <c r="E27" s="30">
         <v>3</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F27" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G27" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C29" s="3">
         <f>0.328 / 10</f>
         <v>3.2800000000000003E-2</v>
       </c>
-      <c r="E25" s="5">
-        <v>0</v>
-      </c>
-      <c r="F25" s="11" t="s">
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G25" s="28" t="s">
+      <c r="G29" s="28" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="11">
-        <v>2</v>
-      </c>
-      <c r="C26" s="3">
+      <c r="B30" s="11">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3">
         <v>0.5</v>
       </c>
-      <c r="D26" s="3">
-        <f>C26*B26</f>
+      <c r="D30" s="3">
+        <f>C30*B30</f>
         <v>1</v>
       </c>
-      <c r="E26" s="5">
-        <v>0</v>
-      </c>
-      <c r="F26" s="22" t="s">
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="29" t="s">
+      <c r="G30" s="29" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="11">
-        <v>2</v>
-      </c>
-      <c r="C27" s="3">
+      <c r="B31" s="11">
+        <v>2</v>
+      </c>
+      <c r="C31" s="3">
         <v>0.7</v>
       </c>
-      <c r="D27" s="3">
-        <f>C27*B27</f>
+      <c r="D31" s="3">
+        <f>C31*B31</f>
         <v>1.4</v>
       </c>
-      <c r="E27" s="5">
-        <v>0</v>
-      </c>
-      <c r="F27" s="22" t="s">
+      <c r="E31" s="5">
+        <v>0</v>
+      </c>
+      <c r="F31" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G31" s="29" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A21:H21"/>
+  <mergeCells count="10">
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A25:H25"/>
     <mergeCell ref="G13:G17"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A24:H24"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="F13:F18"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A21:H21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{590ADCCA-8CE7-40AA-8C96-4A2D1FC3681E}"/>
@@ -1295,17 +1365,17 @@
     <hyperlink ref="G8" r:id="rId4" location="complte_desc" display="https://www.gotronic.fr/art-roulement-19-6-6mm-157.htm - complte_desc" xr:uid="{668C1373-B577-40D7-AE22-CEC46B56C596}"/>
     <hyperlink ref="G18" r:id="rId5" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{8FB5AF53-6074-4AC8-B954-48BA8EAD3BBD}"/>
     <hyperlink ref="G4" r:id="rId6" xr:uid="{5695B478-FFC7-41D3-9378-789EA5284F3B}"/>
-    <hyperlink ref="G22" r:id="rId7" display="https://www.gotronic.fr/art-carte-teensy-3-5-25425.htm" xr:uid="{7F61F742-4E65-43DD-B561-497192D7846D}"/>
+    <hyperlink ref="G26" r:id="rId7" display="https://www.gotronic.fr/art-carte-teensy-3-5-25425.htm" xr:uid="{7F61F742-4E65-43DD-B561-497192D7846D}"/>
     <hyperlink ref="G13:G17" r:id="rId8" display="https://www.makerbeam.com/makerbeam-makerbeam-regular-starter-kit-black.html" xr:uid="{CFD83EBE-9F65-4299-92FF-2460DE3F7642}"/>
-    <hyperlink ref="G23" r:id="rId9" xr:uid="{686BB581-4F17-4F21-B9CD-225D9D0390C3}"/>
-    <hyperlink ref="G25" r:id="rId10" xr:uid="{95571536-5EEA-4D58-947A-37D156F02C8F}"/>
-    <hyperlink ref="G26" r:id="rId11" location="complte_desc" display="https://www.gotronic.fr/art-porte-fusible-mfh250-5805.htm - complte_desc" xr:uid="{2A734C6D-0F87-401B-9A3C-8FDF673C600B}"/>
-    <hyperlink ref="G27" r:id="rId12" xr:uid="{7D60B761-8C23-4981-9078-DE27729C07D0}"/>
+    <hyperlink ref="G27" r:id="rId9" xr:uid="{686BB581-4F17-4F21-B9CD-225D9D0390C3}"/>
+    <hyperlink ref="G29" r:id="rId10" xr:uid="{95571536-5EEA-4D58-947A-37D156F02C8F}"/>
+    <hyperlink ref="G30" r:id="rId11" location="complte_desc" display="https://www.gotronic.fr/art-porte-fusible-mfh250-5805.htm - complte_desc" xr:uid="{2A734C6D-0F87-401B-9A3C-8FDF673C600B}"/>
+    <hyperlink ref="G31" r:id="rId12" xr:uid="{7D60B761-8C23-4981-9078-DE27729C07D0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId13"/>
   <ignoredErrors>
-    <ignoredError sqref="G26:G27" numberStoredAsText="1"/>
+    <ignoredError sqref="G30:G31" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1315,7 +1385,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
maj noms de fichiers meca
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git folder\my_robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFB845C-6BB4-4465-81B2-B7446085BE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52171D4-9C12-40F4-8A05-330D99A275B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
   <si>
     <t>Description</t>
   </si>
@@ -225,9 +225,6 @@
     </r>
   </si>
   <si>
-    <t>Structure MakerBeam</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -278,6 +275,28 @@
   </si>
   <si>
     <t>Étage Lidar</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Microrupteur - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SS-5GL</t>
+    </r>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Structures MakerBeam</t>
   </si>
 </sst>
 </file>
@@ -507,12 +526,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -525,17 +550,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -821,7 +840,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,28 +881,28 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="13" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -912,7 +931,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B5" s="6">
         <v>2</v>
@@ -936,42 +955,39 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="7">
+        <v>7.99</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="11">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B7" s="11">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
         <f>7.9 / 2</f>
         <v>3.95</v>
       </c>
-      <c r="D6" s="3">
-        <f>C6*B6</f>
-        <v>7.9</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="8">
-        <v>32850</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="11">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3">
-        <v>3.2</v>
-      </c>
       <c r="D7" s="3">
         <f>C7*B7</f>
-        <v>6.4</v>
+        <v>7.9</v>
       </c>
       <c r="E7" s="5">
         <v>0</v>
@@ -980,22 +996,22 @@
         <v>26</v>
       </c>
       <c r="G7" s="8">
-        <v>32866</v>
+        <v>32850</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B8" s="11">
         <v>2</v>
       </c>
       <c r="C8" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D8" s="10">
+        <v>3.2</v>
+      </c>
+      <c r="D8" s="3">
         <f>C8*B8</f>
-        <v>2.2000000000000002</v>
+        <v>6.4</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
@@ -1004,23 +1020,39 @@
         <v>26</v>
       </c>
       <c r="G8" s="8">
-        <v>24760</v>
+        <v>32866</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9" s="11">
         <v>2</v>
       </c>
+      <c r="C9" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D9" s="10">
+        <f>C9*B9</f>
+        <v>2.2000000000000002</v>
+      </c>
       <c r="E9" s="5">
         <v>0</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="8">
+        <v>24760</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>30</v>
+      </c>
+      <c r="B10" s="11">
+        <v>2</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
@@ -1028,197 +1060,189 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="34"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B14" s="11">
         <v>4</v>
       </c>
-      <c r="E13" s="5">
-        <v>0</v>
-      </c>
-      <c r="F13" s="34" t="s">
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="32">
-        <v>100012</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="G14" s="39"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="19">
-        <v>2</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="5">
-        <v>0</v>
-      </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="32"/>
-    </row>
-    <row r="15" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="B15" s="19">
+        <v>2</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="39"/>
+    </row>
+    <row r="16" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="19">
-        <v>4</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16">
-        <v>0</v>
-      </c>
-      <c r="F15" s="34"/>
-      <c r="G15" s="32"/>
-    </row>
-    <row r="16" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>49</v>
-      </c>
       <c r="B16" s="19">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="5">
-        <v>0</v>
-      </c>
-      <c r="F16" s="34"/>
-      <c r="G16" s="32"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="36"/>
+      <c r="G16" s="39"/>
+    </row>
+    <row r="17" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="19">
+        <v>2</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="36"/>
+      <c r="G17" s="39"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="11">
-        <v>2</v>
-      </c>
-      <c r="E17" s="5">
-        <v>0</v>
-      </c>
-      <c r="F17" s="34"/>
-      <c r="G17" s="32"/>
-    </row>
-    <row r="18" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="B18" s="11">
+        <v>2</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="36"/>
+      <c r="G18" s="39"/>
+    </row>
+    <row r="19" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="16">
-        <v>0</v>
-      </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="17">
+      <c r="B19" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="16">
+        <v>0</v>
+      </c>
+      <c r="F19" s="36"/>
+      <c r="G19" s="17">
         <v>100315</v>
       </c>
-      <c r="H18" s="14"/>
-    </row>
-    <row r="19" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+    </row>
+    <row r="21" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+    </row>
+    <row r="22" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-    </row>
-    <row r="20" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="37"/>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-    </row>
-    <row r="21" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-    </row>
-    <row r="22" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B22" s="39">
-        <v>2</v>
-      </c>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="40">
-        <f>E15</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
     </row>
     <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="33" t="s">
+      <c r="A24" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="11">
         <v>1</v>
@@ -1247,12 +1271,9 @@
       <c r="B27" s="11">
         <v>2</v>
       </c>
-      <c r="C27" s="3">
-        <v>2.5</v>
-      </c>
+      <c r="C27" s="3"/>
       <c r="D27" s="3">
-        <f>C27*B27</f>
-        <v>5</v>
+        <v>7.49</v>
       </c>
       <c r="E27" s="30">
         <v>3</v>
@@ -1265,23 +1286,23 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
+      <c r="A28" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C29" s="3">
         <f>0.328 / 10</f>
@@ -1291,15 +1312,15 @@
         <v>0</v>
       </c>
       <c r="F29" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" s="28" t="s">
         <v>62</v>
-      </c>
-      <c r="G29" s="28" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B30" s="11">
         <v>2</v>
@@ -1318,12 +1339,12 @@
         <v>26</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" s="11">
         <v>2</v>
@@ -1342,35 +1363,34 @@
         <v>26</v>
       </c>
       <c r="G31" s="29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="A28:H28"/>
     <mergeCell ref="A25:H25"/>
-    <mergeCell ref="G13:G17"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A12:H12"/>
-    <mergeCell ref="F13:F18"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="A13:H13"/>
+    <mergeCell ref="F14:F19"/>
+    <mergeCell ref="A20:H20"/>
+    <mergeCell ref="A22:H22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{590ADCCA-8CE7-40AA-8C96-4A2D1FC3681E}"/>
-    <hyperlink ref="G6" r:id="rId2" display="https://www.gotronic.fr/art-paire-de-moyeux-alu-1998-21781.htm" xr:uid="{244CC552-A9F4-455C-BE90-80AABB27A3FC}"/>
-    <hyperlink ref="G7" r:id="rId3" display="https://www.gotronic.fr/art-roue-libre-3-4-955-21789.htm" xr:uid="{9FA631D8-4924-422F-9436-0F4CC6AD4E31}"/>
-    <hyperlink ref="G8" r:id="rId4" location="complte_desc" display="https://www.gotronic.fr/art-roulement-19-6-6mm-157.htm - complte_desc" xr:uid="{668C1373-B577-40D7-AE22-CEC46B56C596}"/>
-    <hyperlink ref="G18" r:id="rId5" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{8FB5AF53-6074-4AC8-B954-48BA8EAD3BBD}"/>
-    <hyperlink ref="G4" r:id="rId6" xr:uid="{5695B478-FFC7-41D3-9378-789EA5284F3B}"/>
-    <hyperlink ref="G26" r:id="rId7" display="https://www.gotronic.fr/art-carte-teensy-3-5-25425.htm" xr:uid="{7F61F742-4E65-43DD-B561-497192D7846D}"/>
-    <hyperlink ref="G13:G17" r:id="rId8" display="https://www.makerbeam.com/makerbeam-makerbeam-regular-starter-kit-black.html" xr:uid="{CFD83EBE-9F65-4299-92FF-2460DE3F7642}"/>
-    <hyperlink ref="G27" r:id="rId9" xr:uid="{686BB581-4F17-4F21-B9CD-225D9D0390C3}"/>
-    <hyperlink ref="G29" r:id="rId10" xr:uid="{95571536-5EEA-4D58-947A-37D156F02C8F}"/>
-    <hyperlink ref="G30" r:id="rId11" location="complte_desc" display="https://www.gotronic.fr/art-porte-fusible-mfh250-5805.htm - complte_desc" xr:uid="{2A734C6D-0F87-401B-9A3C-8FDF673C600B}"/>
-    <hyperlink ref="G31" r:id="rId12" xr:uid="{7D60B761-8C23-4981-9078-DE27729C07D0}"/>
+    <hyperlink ref="G7" r:id="rId2" display="https://www.gotronic.fr/art-paire-de-moyeux-alu-1998-21781.htm" xr:uid="{244CC552-A9F4-455C-BE90-80AABB27A3FC}"/>
+    <hyperlink ref="G8" r:id="rId3" display="https://www.gotronic.fr/art-roue-libre-3-4-955-21789.htm" xr:uid="{9FA631D8-4924-422F-9436-0F4CC6AD4E31}"/>
+    <hyperlink ref="G9" r:id="rId4" location="complte_desc" display="https://www.gotronic.fr/art-roulement-19-6-6mm-157.htm - complte_desc" xr:uid="{668C1373-B577-40D7-AE22-CEC46B56C596}"/>
+    <hyperlink ref="G4" r:id="rId5" xr:uid="{5695B478-FFC7-41D3-9378-789EA5284F3B}"/>
+    <hyperlink ref="G26" r:id="rId6" display="https://www.gotronic.fr/art-carte-teensy-3-5-25425.htm" xr:uid="{7F61F742-4E65-43DD-B561-497192D7846D}"/>
+    <hyperlink ref="G27" r:id="rId7" xr:uid="{686BB581-4F17-4F21-B9CD-225D9D0390C3}"/>
+    <hyperlink ref="G29" r:id="rId8" xr:uid="{95571536-5EEA-4D58-947A-37D156F02C8F}"/>
+    <hyperlink ref="G30" r:id="rId9" location="complte_desc" display="https://www.gotronic.fr/art-porte-fusible-mfh250-5805.htm - complte_desc" xr:uid="{2A734C6D-0F87-401B-9A3C-8FDF673C600B}"/>
+    <hyperlink ref="G31" r:id="rId10" xr:uid="{7D60B761-8C23-4981-9078-DE27729C07D0}"/>
+    <hyperlink ref="G6" r:id="rId11" location="customerReviews" xr:uid="{C22BA633-0DDD-43D0-80A9-998910C51761}"/>
+    <hyperlink ref="G19" r:id="rId12" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{8FB5AF53-6074-4AC8-B954-48BA8EAD3BBD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId13"/>
@@ -1427,17 +1447,17 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1533,10 +1553,10 @@
       <c r="D6" s="5">
         <v>0</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="35"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="1" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
creation projet sur platformIO
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git folder\my_robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52171D4-9C12-40F4-8A05-330D99A275B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA8CBA1-39CE-48A3-A84A-55A20B506AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="89">
   <si>
     <t>Description</t>
   </si>
@@ -189,9 +189,6 @@
   </si>
   <si>
     <t>Profilé MakerBeam 200mm</t>
-  </si>
-  <si>
-    <t>Modules</t>
   </si>
   <si>
     <t>nRF24L01</t>
@@ -225,13 +222,7 @@
     </r>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Connecteurs</t>
-  </si>
-  <si>
-    <t>Embase à broches Molex, KK 254, 4 pôles</t>
   </si>
   <si>
     <t>RS</t>
@@ -297,6 +288,60 @@
   </si>
   <si>
     <t>Structures MakerBeam</t>
+  </si>
+  <si>
+    <t>TSR 1-2450</t>
+  </si>
+  <si>
+    <t>666-4379</t>
+  </si>
+  <si>
+    <t>Embase Weidmüller SL 3.50/02/180G</t>
+  </si>
+  <si>
+    <t>Embase Molex KK 254 - 4 pôles</t>
+  </si>
+  <si>
+    <t>Batterie BAKTH 7.2V 4000mAh NiMH</t>
+  </si>
+  <si>
+    <t>Composants passifs</t>
+  </si>
+  <si>
+    <t>Diode traversante</t>
+  </si>
+  <si>
+    <t>Bornier Weidmüller BL 3.50/02/180</t>
+  </si>
+  <si>
+    <t>171-657</t>
+  </si>
+  <si>
+    <t>171-499</t>
+  </si>
+  <si>
+    <t>Adaptateur connecteur Tamiya</t>
+  </si>
+  <si>
+    <t>Résistance traversante 390k</t>
+  </si>
+  <si>
+    <t>Résistance traversante 100k</t>
+  </si>
+  <si>
+    <t>Résistance traversante 500</t>
+  </si>
+  <si>
+    <t>Résistance traversante 4,7k</t>
+  </si>
+  <si>
+    <t>Résistance traversante 1k</t>
+  </si>
+  <si>
+    <t>Condensateur 100µ</t>
+  </si>
+  <si>
+    <t>Condensateur 10µ</t>
   </si>
 </sst>
 </file>
@@ -438,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -535,6 +580,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -550,11 +604,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -837,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -881,32 +947,32 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="13" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="A2" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:8" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="11">
         <v>2</v>
@@ -918,8 +984,8 @@
         <f>C4*B4</f>
         <v>25.98</v>
       </c>
-      <c r="E4" s="5">
-        <v>1</v>
+      <c r="E4" s="30">
+        <v>2</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>48</v>
@@ -931,7 +997,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B5" s="6">
         <v>2</v>
@@ -955,7 +1021,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B6" s="6">
         <v>4</v>
@@ -964,8 +1030,8 @@
       <c r="D6" s="7">
         <v>7.99</v>
       </c>
-      <c r="E6" s="5">
-        <v>0</v>
+      <c r="E6" s="30">
+        <v>5</v>
       </c>
       <c r="F6" s="31" t="s">
         <v>48</v>
@@ -976,10 +1042,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C7" s="3">
         <f>7.9 / 2</f>
@@ -987,10 +1053,10 @@
       </c>
       <c r="D7" s="3">
         <f>C7*B7</f>
-        <v>7.9</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
+        <v>15.8</v>
+      </c>
+      <c r="E7" s="30">
+        <v>4</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>26</v>
@@ -1013,8 +1079,8 @@
         <f>C8*B8</f>
         <v>6.4</v>
       </c>
-      <c r="E8" s="5">
-        <v>0</v>
+      <c r="E8" s="30">
+        <v>2</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>26</v>
@@ -1037,8 +1103,8 @@
         <f>C9*B9</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="E9" s="5">
-        <v>0</v>
+      <c r="E9" s="30">
+        <v>2</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>26</v>
@@ -1062,8 +1128,8 @@
       <c r="A11" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="40" t="s">
-        <v>72</v>
+      <c r="B11" s="35" t="s">
+        <v>69</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
@@ -1071,7 +1137,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -1080,303 +1146,530 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="36">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3">
+        <v>23.99</v>
+      </c>
+      <c r="D13" s="3">
+        <f xml:space="preserve"> B13*C13</f>
+        <v>47.98</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="36">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="30">
+        <v>2</v>
+      </c>
+      <c r="F14" s="36"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B16" s="11">
         <v>4</v>
       </c>
-      <c r="E14" s="5">
-        <v>0</v>
-      </c>
-      <c r="F14" s="36" t="s">
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="G14" s="39"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="G16" s="34"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="19">
-        <v>2</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="5">
-        <v>0</v>
-      </c>
-      <c r="F15" s="36"/>
-      <c r="G15" s="39"/>
-    </row>
-    <row r="16" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="B17" s="19">
+        <v>2</v>
+      </c>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="39"/>
+      <c r="G17" s="34"/>
+    </row>
+    <row r="18" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B18" s="19">
         <v>8</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16">
-        <v>0</v>
-      </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="39"/>
-    </row>
-    <row r="17" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16">
+        <v>0</v>
+      </c>
+      <c r="F18" s="39"/>
+      <c r="G18" s="34"/>
+    </row>
+    <row r="19" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="19">
-        <v>2</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="5">
-        <v>0</v>
-      </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="39"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B19" s="19">
+        <v>2</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="5">
+        <v>0</v>
+      </c>
+      <c r="F19" s="39"/>
+      <c r="G19" s="34"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="11">
-        <v>2</v>
-      </c>
-      <c r="E18" s="5">
-        <v>0</v>
-      </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="39"/>
-    </row>
-    <row r="19" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="B20" s="11">
+        <v>2</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0</v>
+      </c>
+      <c r="F20" s="39"/>
+      <c r="G20" s="34"/>
+    </row>
+    <row r="21" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B21" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="16">
+        <v>0</v>
+      </c>
+      <c r="F21" s="39"/>
+      <c r="G21" s="17">
+        <v>100315</v>
+      </c>
+      <c r="H21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="37"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+    </row>
+    <row r="23" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+    </row>
+    <row r="24" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="37"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+    </row>
+    <row r="26" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="11">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>29.7</v>
+      </c>
+      <c r="D27" s="3">
+        <f>C27*B27</f>
+        <v>29.7</v>
+      </c>
+      <c r="E27" s="30">
+        <v>1</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="8">
+        <v>34778</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="11">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3">
+        <v>7.49</v>
+      </c>
+      <c r="E28" s="30">
+        <v>3</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="36">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3">
+        <v>6.72</v>
+      </c>
+      <c r="D29" s="3">
+        <f xml:space="preserve"> 1*C29</f>
+        <v>6.72</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="16">
-        <v>0</v>
-      </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="17">
-        <v>100315</v>
-      </c>
-      <c r="H19" s="14"/>
-    </row>
-    <row r="20" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="36">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="28"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="36">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="28"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="36">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="28"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="36">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="5">
+        <v>0</v>
+      </c>
+      <c r="F34" s="36"/>
+      <c r="G34" s="28"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="36">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="5">
+        <v>0</v>
+      </c>
+      <c r="F35" s="36"/>
+      <c r="G35" s="28"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="36">
+        <v>6</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="46">
+        <v>2</v>
+      </c>
+      <c r="F36" s="36"/>
+      <c r="G36" s="28"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" s="36">
+        <v>4</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="5">
+        <v>0</v>
+      </c>
+      <c r="F37" s="36"/>
+      <c r="G37" s="28"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="36">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="5">
+        <v>0</v>
+      </c>
+      <c r="F38" s="36"/>
+      <c r="G38" s="28"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="37"/>
+      <c r="C39" s="37"/>
+      <c r="D39" s="37"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+    </row>
+    <row r="40" spans="1:8" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="42">
+        <v>2</v>
+      </c>
+      <c r="C40" s="44">
+        <v>1.2410000000000001</v>
+      </c>
+      <c r="D40" s="44">
+        <f>B40*C40</f>
+        <v>2.4820000000000002</v>
+      </c>
+      <c r="E40" s="45">
+        <v>0</v>
+      </c>
+      <c r="F40" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="G40" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="H40" s="42"/>
+    </row>
+    <row r="41" spans="1:8" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="42">
+        <v>2</v>
+      </c>
+      <c r="C41" s="44">
+        <v>1.51</v>
+      </c>
+      <c r="D41" s="44">
+        <f>B41*C41</f>
+        <v>3.02</v>
+      </c>
+      <c r="E41" s="46">
+        <v>2</v>
+      </c>
+      <c r="F41" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="G41" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="H41" s="42"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-    </row>
-    <row r="21" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-    </row>
-    <row r="22" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-    </row>
-    <row r="24" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B26" s="11">
-        <v>1</v>
-      </c>
-      <c r="C26" s="3">
-        <v>29.7</v>
-      </c>
-      <c r="D26" s="3">
-        <f>C26*B26</f>
-        <v>29.7</v>
-      </c>
-      <c r="E26" s="5">
-        <v>0</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G26" s="8">
-        <v>34778</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="11">
-        <v>2</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3">
-        <v>7.49</v>
-      </c>
-      <c r="E27" s="30">
-        <v>3</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="3">
+      <c r="C42" s="3">
         <f>0.328 / 10</f>
         <v>3.2800000000000003E-2</v>
       </c>
-      <c r="E29" s="5">
-        <v>0</v>
-      </c>
-      <c r="F29" s="11" t="s">
+      <c r="E42" s="5">
+        <v>0</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G42" s="28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="11">
+        <v>1</v>
+      </c>
+      <c r="C43" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D43" s="3">
+        <f>C43*B43</f>
+        <v>0.5</v>
+      </c>
+      <c r="E43" s="30">
+        <v>2</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G43" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B44" s="11">
+        <v>1</v>
+      </c>
+      <c r="C44" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="D44" s="3">
+        <f>C44*B44</f>
+        <v>0.7</v>
+      </c>
+      <c r="E44" s="30">
+        <v>2</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G44" s="29" t="s">
         <v>63</v>
-      </c>
-      <c r="B30" s="11">
-        <v>2</v>
-      </c>
-      <c r="C30" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D30" s="3">
-        <f>C30*B30</f>
-        <v>1</v>
-      </c>
-      <c r="E30" s="5">
-        <v>0</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="G30" s="29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="11">
-        <v>2</v>
-      </c>
-      <c r="C31" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="D31" s="3">
-        <f>C31*B31</f>
-        <v>1.4</v>
-      </c>
-      <c r="E31" s="5">
-        <v>0</v>
-      </c>
-      <c r="F31" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="29" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A39:H39"/>
     <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="F16:F21"/>
+    <mergeCell ref="A22:H22"/>
     <mergeCell ref="A24:H24"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A13:H13"/>
-    <mergeCell ref="F14:F19"/>
-    <mergeCell ref="A20:H20"/>
-    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A30:H30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{590ADCCA-8CE7-40AA-8C96-4A2D1FC3681E}"/>
@@ -1384,18 +1677,22 @@
     <hyperlink ref="G8" r:id="rId3" display="https://www.gotronic.fr/art-roue-libre-3-4-955-21789.htm" xr:uid="{9FA631D8-4924-422F-9436-0F4CC6AD4E31}"/>
     <hyperlink ref="G9" r:id="rId4" location="complte_desc" display="https://www.gotronic.fr/art-roulement-19-6-6mm-157.htm - complte_desc" xr:uid="{668C1373-B577-40D7-AE22-CEC46B56C596}"/>
     <hyperlink ref="G4" r:id="rId5" xr:uid="{5695B478-FFC7-41D3-9378-789EA5284F3B}"/>
-    <hyperlink ref="G26" r:id="rId6" display="https://www.gotronic.fr/art-carte-teensy-3-5-25425.htm" xr:uid="{7F61F742-4E65-43DD-B561-497192D7846D}"/>
-    <hyperlink ref="G27" r:id="rId7" xr:uid="{686BB581-4F17-4F21-B9CD-225D9D0390C3}"/>
-    <hyperlink ref="G29" r:id="rId8" xr:uid="{95571536-5EEA-4D58-947A-37D156F02C8F}"/>
-    <hyperlink ref="G30" r:id="rId9" location="complte_desc" display="https://www.gotronic.fr/art-porte-fusible-mfh250-5805.htm - complte_desc" xr:uid="{2A734C6D-0F87-401B-9A3C-8FDF673C600B}"/>
-    <hyperlink ref="G31" r:id="rId10" xr:uid="{7D60B761-8C23-4981-9078-DE27729C07D0}"/>
+    <hyperlink ref="G27" r:id="rId6" display="https://www.gotronic.fr/art-carte-teensy-3-5-25425.htm" xr:uid="{7F61F742-4E65-43DD-B561-497192D7846D}"/>
+    <hyperlink ref="G28" r:id="rId7" xr:uid="{686BB581-4F17-4F21-B9CD-225D9D0390C3}"/>
+    <hyperlink ref="G42" r:id="rId8" xr:uid="{95571536-5EEA-4D58-947A-37D156F02C8F}"/>
+    <hyperlink ref="G43" r:id="rId9" location="complte_desc" display="https://www.gotronic.fr/art-porte-fusible-mfh250-5805.htm - complte_desc" xr:uid="{2A734C6D-0F87-401B-9A3C-8FDF673C600B}"/>
+    <hyperlink ref="G44" r:id="rId10" xr:uid="{7D60B761-8C23-4981-9078-DE27729C07D0}"/>
     <hyperlink ref="G6" r:id="rId11" location="customerReviews" xr:uid="{C22BA633-0DDD-43D0-80A9-998910C51761}"/>
-    <hyperlink ref="G19" r:id="rId12" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{8FB5AF53-6074-4AC8-B954-48BA8EAD3BBD}"/>
+    <hyperlink ref="G21" r:id="rId12" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{8FB5AF53-6074-4AC8-B954-48BA8EAD3BBD}"/>
+    <hyperlink ref="G29" r:id="rId13" xr:uid="{E8D72A56-4E65-41EC-AE9F-8314F8ADC261}"/>
+    <hyperlink ref="G13" r:id="rId14" xr:uid="{8979B7EA-02BC-444A-B8BE-96152DE16CEE}"/>
+    <hyperlink ref="G41" r:id="rId15" xr:uid="{4A4E886E-F8EE-427F-B2B2-2C332F5521F2}"/>
+    <hyperlink ref="G40" r:id="rId16" xr:uid="{38243AFD-FCED-4066-88E4-3E67A6808F3F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId17"/>
   <ignoredErrors>
-    <ignoredError sqref="G30:G31" numberStoredAsText="1"/>
+    <ignoredError sqref="G43:G44" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1447,17 +1744,17 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1553,10 +1850,10 @@
       <c r="D6" s="5">
         <v>0</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="37"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="1" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
ajout trous vis bloc moteurs chassis
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git folder\my_robot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Folder\my_robot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{271AA8C0-2C0E-4949-BAC2-AD280810F9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC149B1-EF1C-4AA4-9D2D-5A80AC25DBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Éléments achetés" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -528,12 +528,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -580,9 +574,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -617,6 +608,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -902,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,54 +915,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="25" t="s">
+      <c r="C1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="13" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="1:8" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -981,7 +978,7 @@
         <f>C4*B4</f>
         <v>25.98</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="28">
         <v>2</v>
       </c>
       <c r="F4" s="11" t="s">
@@ -1006,7 +1003,7 @@
         <f>C5*B5</f>
         <v>38.380000000000003</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="28">
         <v>2</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -1027,10 +1024,10 @@
       <c r="D6" s="7">
         <v>7.99</v>
       </c>
-      <c r="E6" s="30">
+      <c r="E6" s="28">
         <v>5</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="29" t="s">
         <v>48</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -1052,7 +1049,7 @@
         <f>C7*B7</f>
         <v>15.8</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="28">
         <v>4</v>
       </c>
       <c r="F7" s="11" t="s">
@@ -1076,7 +1073,7 @@
         <f>C8*B8</f>
         <v>6.4</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="28">
         <v>2</v>
       </c>
       <c r="F8" s="11" t="s">
@@ -1100,7 +1097,7 @@
         <f>C9*B9</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="28">
         <v>2</v>
       </c>
       <c r="F9" s="11" t="s">
@@ -1117,15 +1114,15 @@
       <c r="B10" s="11">
         <v>2</v>
       </c>
-      <c r="E10" s="5">
-        <v>0</v>
+      <c r="E10" s="28">
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="32" t="s">
         <v>69</v>
       </c>
       <c r="E11" s="5">
@@ -1138,15 +1135,13 @@
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="5">
-        <v>0</v>
-      </c>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>75</v>
       </c>
-      <c r="B13" s="36">
+      <c r="B13" s="33">
         <v>2</v>
       </c>
       <c r="C13" s="3">
@@ -1156,10 +1151,10 @@
         <f xml:space="preserve"> B13*C13</f>
         <v>47.98</v>
       </c>
-      <c r="E13" s="30">
-        <v>2</v>
-      </c>
-      <c r="F13" s="36" t="s">
+      <c r="E13" s="28">
+        <v>2</v>
+      </c>
+      <c r="F13" s="33" t="s">
         <v>48</v>
       </c>
       <c r="G13" s="8" t="s">
@@ -1170,28 +1165,28 @@
       <c r="A14" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="33">
         <v>2</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="30">
-        <v>2</v>
-      </c>
-      <c r="F14" s="36"/>
+      <c r="E14" s="28">
+        <v>2</v>
+      </c>
+      <c r="F14" s="33"/>
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1200,58 +1195,60 @@
       <c r="B16" s="11">
         <v>4</v>
       </c>
-      <c r="E16" s="5">
-        <v>0</v>
-      </c>
-      <c r="F16" s="44" t="s">
+      <c r="E16" s="28">
+        <v>4</v>
+      </c>
+      <c r="F16" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="34"/>
+      <c r="G16" s="45">
+        <v>100315</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="19">
-        <v>2</v>
-      </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="5">
-        <v>0</v>
-      </c>
-      <c r="F17" s="44"/>
-      <c r="G17" s="34"/>
-    </row>
-    <row r="18" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="B17" s="17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="28">
+        <v>8</v>
+      </c>
+      <c r="F17" s="41"/>
+      <c r="G17" s="45"/>
+    </row>
+    <row r="18" spans="1:8" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="17">
         <v>8</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
-      <c r="E18" s="16">
-        <v>0</v>
-      </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="34"/>
-    </row>
-    <row r="19" spans="1:8" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="44">
+        <v>6</v>
+      </c>
+      <c r="F18" s="41"/>
+      <c r="G18" s="45"/>
+    </row>
+    <row r="19" spans="1:8" s="16" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="17">
         <v>2</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
-      <c r="E19" s="5">
-        <v>0</v>
-      </c>
-      <c r="F19" s="44"/>
-      <c r="G19" s="34"/>
+      <c r="E19" s="28">
+        <v>8</v>
+      </c>
+      <c r="F19" s="41"/>
+      <c r="G19" s="45"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1260,78 +1257,76 @@
       <c r="B20" s="11">
         <v>2</v>
       </c>
-      <c r="E20" s="5">
-        <v>0</v>
-      </c>
-      <c r="F20" s="44"/>
-      <c r="G20" s="34"/>
-    </row>
-    <row r="21" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E20" s="28">
+        <v>8</v>
+      </c>
+      <c r="F20" s="41"/>
+      <c r="G20" s="45"/>
+    </row>
+    <row r="21" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="19" t="s">
         <v>69</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
-      <c r="E21" s="16">
-        <v>0</v>
-      </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="17">
-        <v>100315</v>
-      </c>
+      <c r="E21" s="44">
+        <v>12</v>
+      </c>
+      <c r="F21" s="41"/>
+      <c r="G21" s="45"/>
       <c r="H21" s="14"/>
     </row>
-    <row r="22" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="s">
+    <row r="22" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-    </row>
-    <row r="23" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-    </row>
-    <row r="24" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="42" t="s">
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+    </row>
+    <row r="23" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="30"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+    </row>
+    <row r="24" spans="1:8" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
     </row>
     <row r="26" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="21" t="s">
         <v>64</v>
       </c>
       <c r="B27" s="11">
@@ -1344,7 +1339,7 @@
         <f>C27*B27</f>
         <v>29.7</v>
       </c>
-      <c r="E27" s="30">
+      <c r="E27" s="28">
         <v>1</v>
       </c>
       <c r="F27" s="11" t="s">
@@ -1365,7 +1360,7 @@
       <c r="D28" s="3">
         <v>7.49</v>
       </c>
-      <c r="E28" s="30">
+      <c r="E28" s="28">
         <v>3</v>
       </c>
       <c r="F28" s="11" t="s">
@@ -1379,7 +1374,7 @@
       <c r="A29" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="36">
+      <c r="B29" s="33">
         <v>1</v>
       </c>
       <c r="C29" s="3">
@@ -1392,196 +1387,196 @@
       <c r="E29" s="5">
         <v>0</v>
       </c>
-      <c r="F29" s="36" t="s">
+      <c r="F29" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="G29" s="28" t="s">
+      <c r="G29" s="26" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="42" t="s">
+      <c r="A30" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="36">
+      <c r="B31" s="33">
         <v>1</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="28"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="36">
+      <c r="B32" s="33">
         <v>2</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="28"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="26"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="36">
+      <c r="B33" s="33">
         <v>1</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="28"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="26"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="36">
+      <c r="B34" s="33">
         <v>1</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="5"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="28"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="26"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="36">
+      <c r="B35" s="33">
         <v>1</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="5"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="28"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="26"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B36" s="36">
+      <c r="B36" s="33">
         <v>6</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="28"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="26"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B37" s="36">
+      <c r="B37" s="33">
         <v>4</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="5"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="28"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="26"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="36">
+      <c r="B38" s="33">
         <v>1</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="5"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="28"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="26"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="42" t="s">
+      <c r="A39" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="42"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="42"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="42"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="42"/>
-    </row>
-    <row r="40" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="23" t="s">
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+    </row>
+    <row r="40" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="37">
-        <v>2</v>
-      </c>
-      <c r="C40" s="39">
+      <c r="B40" s="34">
+        <v>2</v>
+      </c>
+      <c r="C40" s="36">
         <v>1.2410000000000001</v>
       </c>
-      <c r="D40" s="39">
+      <c r="D40" s="36">
         <f>B40*C40</f>
         <v>2.4820000000000002</v>
       </c>
-      <c r="E40" s="40">
-        <v>2</v>
-      </c>
-      <c r="F40" s="37" t="s">
+      <c r="E40" s="37">
+        <v>2</v>
+      </c>
+      <c r="F40" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="G40" s="41" t="s">
+      <c r="G40" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="H40" s="37"/>
-    </row>
-    <row r="41" spans="1:8" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="23" t="s">
+      <c r="H40" s="34"/>
+    </row>
+    <row r="41" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="B41" s="37">
-        <v>2</v>
-      </c>
-      <c r="C41" s="39">
+      <c r="B41" s="34">
+        <v>2</v>
+      </c>
+      <c r="C41" s="36">
         <v>1.51</v>
       </c>
-      <c r="D41" s="39">
+      <c r="D41" s="36">
         <f>B41*C41</f>
         <v>3.02</v>
       </c>
-      <c r="E41" s="40">
-        <v>2</v>
-      </c>
-      <c r="F41" s="37" t="s">
+      <c r="E41" s="37">
+        <v>2</v>
+      </c>
+      <c r="F41" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="G41" s="41" t="s">
+      <c r="G41" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="H41" s="37"/>
+      <c r="H41" s="34"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="21" t="s">
+      <c r="B42" s="19" t="s">
         <v>69</v>
       </c>
       <c r="C42" s="3">
@@ -1594,7 +1589,7 @@
       <c r="F42" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G42" s="28" t="s">
+      <c r="G42" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1612,13 +1607,13 @@
         <f>C43*B43</f>
         <v>0.5</v>
       </c>
-      <c r="E43" s="30">
-        <v>2</v>
-      </c>
-      <c r="F43" s="22" t="s">
+      <c r="E43" s="28">
+        <v>2</v>
+      </c>
+      <c r="F43" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="G43" s="29" t="s">
+      <c r="G43" s="27" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1636,18 +1631,18 @@
         <f>C44*B44</f>
         <v>0.7</v>
       </c>
-      <c r="E44" s="30">
-        <v>2</v>
-      </c>
-      <c r="F44" s="22" t="s">
+      <c r="E44" s="28">
+        <v>2</v>
+      </c>
+      <c r="F44" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="G44" s="29" t="s">
+      <c r="G44" s="27" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A39:H39"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A26:H26"/>
@@ -1657,6 +1652,7 @@
     <mergeCell ref="A22:H22"/>
     <mergeCell ref="A24:H24"/>
     <mergeCell ref="A30:H30"/>
+    <mergeCell ref="G16:G21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{590ADCCA-8CE7-40AA-8C96-4A2D1FC3681E}"/>
@@ -1670,7 +1666,7 @@
     <hyperlink ref="G43" r:id="rId9" location="complte_desc" display="https://www.gotronic.fr/art-porte-fusible-mfh250-5805.htm - complte_desc" xr:uid="{2A734C6D-0F87-401B-9A3C-8FDF673C600B}"/>
     <hyperlink ref="G44" r:id="rId10" xr:uid="{7D60B761-8C23-4981-9078-DE27729C07D0}"/>
     <hyperlink ref="G6" r:id="rId11" location="customerReviews" xr:uid="{C22BA633-0DDD-43D0-80A9-998910C51761}"/>
-    <hyperlink ref="G21" r:id="rId12" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{8FB5AF53-6074-4AC8-B954-48BA8EAD3BBD}"/>
+    <hyperlink ref="G16" r:id="rId12" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{8FB5AF53-6074-4AC8-B954-48BA8EAD3BBD}"/>
     <hyperlink ref="G29" r:id="rId13" xr:uid="{E8D72A56-4E65-41EC-AE9F-8314F8ADC261}"/>
     <hyperlink ref="G13" r:id="rId14" xr:uid="{8979B7EA-02BC-444A-B8BE-96152DE16CEE}"/>
     <hyperlink ref="G41" r:id="rId15" xr:uid="{4A4E886E-F8EE-427F-B2B2-2C332F5521F2}"/>
@@ -1702,46 +1698,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1837,10 +1833,10 @@
       <c r="D6" s="5">
         <v>0</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="45"/>
+      <c r="F6" s="42"/>
       <c r="G6" s="1" t="s">
         <v>33</v>
       </c>

</xml_diff>